<commit_message>
Updated Lab01 once againnn
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\ANUL 3\SEM 2\VVSS\LAB\1\CheckLists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\ANUL 3\SEM 2\VVSS\LAB\Proiecte\03_PizzaShop\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" tabRatio="650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="97">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -141,9 +141,6 @@
     <t>R05</t>
   </si>
   <si>
-    <t>R06</t>
-  </si>
-  <si>
     <t>R07</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>In fisier ar trebui salvate si detaliile comenzii pentru care s-a efectuat plata</t>
   </si>
   <si>
-    <t>Vag mentionate</t>
-  </si>
-  <si>
     <t>Nu este mentionata platforma aplicatiei</t>
   </si>
   <si>
@@ -177,27 +171,12 @@
     <t>A02</t>
   </si>
   <si>
-    <t>A03</t>
-  </si>
-  <si>
-    <t>A04</t>
-  </si>
-  <si>
     <t>A05</t>
   </si>
   <si>
-    <t>A06</t>
-  </si>
-  <si>
     <t>A07</t>
   </si>
   <si>
-    <t>A08</t>
-  </si>
-  <si>
-    <t>A09</t>
-  </si>
-  <si>
     <t>30m</t>
   </si>
   <si>
@@ -306,42 +285,21 @@
     <t>Nu exista partitionare pe package-uri</t>
   </si>
   <si>
-    <t>Nu avem clasa Order</t>
-  </si>
-  <si>
-    <t>Lipseste clasa Order si OrderRepository</t>
-  </si>
-  <si>
     <t>Nu se specifica o metoda de tratare a erorilor</t>
   </si>
   <si>
-    <t>Nu au fost considerate</t>
-  </si>
-  <si>
     <t>Denumirea nu este suficient de sugestiva - PaymentAlert, MenuDataModel</t>
   </si>
   <si>
-    <t>Nu avem descrieri</t>
-  </si>
-  <si>
-    <t>Nu avem suficiente denumiri</t>
-  </si>
-  <si>
     <t>C01</t>
   </si>
   <si>
-    <t>C02</t>
-  </si>
-  <si>
     <t>C03</t>
   </si>
   <si>
     <t>In clasele MenuRepository, PaymentRepository avem if (line==null|| line.equals("")) ,unde nu este necesar line==null</t>
   </si>
   <si>
-    <t>Nu avem branching</t>
-  </si>
-  <si>
     <t>Exista in clasa KitchenGUIController</t>
   </si>
   <si>
@@ -349,6 +307,12 @@
   </si>
   <si>
     <t>line39/line41</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>Nu exista mesaje de eroare la aparitia erorilor</t>
   </si>
 </sst>
 </file>
@@ -565,6 +529,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -606,15 +579,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,8 +889,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,19 +910,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -982,10 +946,10 @@
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="26"/>
+      <c r="E4" s="29"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1000,10 +964,10 @@
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="31"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1019,15 +983,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1044,82 +1008,78 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="38">
+      <c r="B10" s="24">
         <v>1</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="39" t="s">
-        <v>41</v>
+      <c r="D10" s="23"/>
+      <c r="E10" s="25" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="38">
+      <c r="B11" s="24">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="39" t="s">
-        <v>42</v>
+      <c r="D11" s="23"/>
+      <c r="E11" s="25" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="38">
+      <c r="B12" s="24">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="39" t="s">
+      <c r="D12" s="23"/>
+      <c r="E12" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="24">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="38">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="37" t="s">
+      <c r="E13" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="39" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="24">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="25"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="24">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="25" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="38">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="38">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="39" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1221,7 +1181,7 @@
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1246,7 +1206,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1265,19 +1225,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1301,10 +1261,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1319,10 +1279,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="34"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1338,15 +1298,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1363,120 +1323,100 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="38">
+      <c r="B10" s="24">
         <v>1</v>
       </c>
-      <c r="C10" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39" t="s">
-        <v>92</v>
+      <c r="C10" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="38">
+      <c r="B11" s="24">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39" t="s">
-        <v>93</v>
+      <c r="C11" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="38">
+      <c r="B12" s="24">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="39" t="s">
-        <v>94</v>
-      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="25"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="38">
+      <c r="B13" s="24">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="39" t="s">
-        <v>95</v>
-      </c>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="38">
+      <c r="B14" s="24">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39" t="s">
-        <v>96</v>
+      <c r="C14" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="38">
+      <c r="B15" s="24">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="39" t="s">
-        <v>97</v>
-      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="25"/>
     </row>
     <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="38">
+      <c r="B16" s="24">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39" t="s">
-        <v>98</v>
+      <c r="C16" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="38">
+      <c r="B17" s="24">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39" t="s">
-        <v>99</v>
-      </c>
+      <c r="C17" s="23"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="38">
+      <c r="B18" s="24">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="39" t="s">
-        <v>100</v>
-      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="25"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
@@ -1559,7 +1499,7 @@
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1584,7 +1524,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1604,19 +1544,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1640,10 +1580,10 @@
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="35"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1658,10 +1598,10 @@
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="37"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1677,15 +1617,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1702,45 +1642,45 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B10" s="38">
+      <c r="B10" s="24">
         <v>1</v>
       </c>
-      <c r="C10" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>104</v>
+      <c r="C10" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="38">
+      <c r="B11" s="24">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="39" t="s">
-        <v>105</v>
+      <c r="C11" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="25" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="38">
+      <c r="B12" s="24">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>106</v>
+      <c r="C12" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1914,7 +1854,7 @@
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1938,7 +1878,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1960,19 +1900,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1996,8 +1936,8 @@
       <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -2012,8 +1952,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -2029,8 +1969,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
       <c r="F6" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2051,182 +1991,182 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B10" s="38">
+      <c r="B10" s="24">
         <v>1</v>
       </c>
-      <c r="C10" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="39" t="s">
-        <v>59</v>
+      <c r="C10" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="38">
+      <c r="B11" s="24">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="39" t="s">
-        <v>66</v>
+      <c r="C11" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="38">
+      <c r="B12" s="24">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="24">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B14" s="24">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="38">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="37" t="s">
+    </row>
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="24">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="39" t="s">
+      <c r="D15" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="39" t="s">
+      <c r="F15" s="25" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B14" s="38">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="39" t="s">
+    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B16" s="24">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C16" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="D16" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="39" t="s">
+      <c r="F16" s="25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="38">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C15" s="37" t="s">
+    <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="24">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D17" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="24">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C18" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="39" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="38">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C16" s="37" t="s">
+      <c r="D18" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="24">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C19" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="39" t="s">
+      <c r="D19" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="39" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="38">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C17" s="37" t="s">
+      <c r="E19" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="39" t="s">
+      <c r="F19" s="25" t="s">
         <v>83</v>
-      </c>
-      <c r="F17" s="39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="38">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" s="39" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="38">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C19" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="F19" s="39" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -2343,11 +2283,11 @@
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
+      <c r="C32" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
       <c r="F32" s="19"/>
     </row>
   </sheetData>

</xml_diff>